<commit_message>
global producr attr removed
</commit_message>
<xml_diff>
--- a/public/assets/uploads/global_products.xlsx
+++ b/public/assets/uploads/global_products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\binu\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FE501B4-CF7A-4A78-88A7-CAC562BED9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5356353-D706-4620-B5C7-4BF8354A5839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{48150E63-6D43-41DE-A9B9-E9B78915DB1A}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Product Name</t>
   </si>
@@ -53,12 +52,6 @@
   </si>
   <si>
     <t>Product Brand</t>
-  </si>
-  <si>
-    <t>Attribute Group</t>
-  </si>
-  <si>
-    <t>Attribute Value</t>
   </si>
   <si>
     <t>Product Category</t>
@@ -428,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E88E40-567D-4DE1-A430-FBDE288D5CC7}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,14 +437,12 @@
     <col min="7" max="7" width="15.7109375" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="13" width="16.85546875" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" customWidth="1"/>
-    <col min="15" max="15" width="49.5703125" customWidth="1"/>
+    <col min="10" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="49.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,16 +474,10 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>